<commit_message>
Update UseCase Format, Tạo UseCase Diagram, Activity Diagram
Update QLNV, Tìm kiếm, Quản lí kho
Tạo UseCase Diagram Tìm kiếm, Quản lí kho
Tạo Activity Diagram Quản lí kho
</commit_message>
<xml_diff>
--- a/Phân tích/UseCases/1. QLNV + 2. Chấm công.xlsx
+++ b/Phân tích/UseCases/1. QLNV + 2. Chấm công.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CNPM\Phân tích\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Phân tích\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC02D99E-869E-4B34-B386-FB49DDE19582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BEAD05-27F8-490A-B963-F298EC8EC401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{70C1F1DC-1DC4-47AB-BCD1-D42F388C200A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70C1F1DC-1DC4-47AB-BCD1-D42F388C200A}"/>
   </bookViews>
   <sheets>
     <sheet name="UCFormat -QLNV" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="112">
   <si>
     <t>Use Case Number:</t>
   </si>
@@ -103,19 +103,6 @@
     <t>3. Actor chọn chức năng quản lí nhân viên</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>Actor có thể chọn xem bảng đánh giá nhân viên</t>
-    </r>
-  </si>
-  <si>
     <t>Actor có đủ quyền hạn.</t>
   </si>
   <si>
@@ -131,57 +118,7 @@
     <t>Date:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4. Hệ thống chuyển tiếp vào trang danh mục nhân viên, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>A1.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. Actor chọn xem thông tin nhân viên. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>A2.</t>
-    </r>
-  </si>
-  <si>
     <t>6. Hệ thống hiển thị cửa sổ thông tin nhân viên.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">7. Actor xem cửa sổ đã hiển thị </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>A3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t xml:space="preserve">, use case kết thúc tại đây. </t>
-    </r>
   </si>
   <si>
     <t>1. Actor nhấn nút Thêm nhân viên</t>
@@ -228,12 +165,6 @@
     <t>5. Hệ thống cập nhật thông tin nhân viên vào cơ sở dữ liệu, hiện thông báo "Cập nhật thành công".</t>
   </si>
   <si>
-    <t>1. Actor quản lí nhấn vào nút Hủy</t>
-  </si>
-  <si>
-    <t>2. Hệ thống quay về bước 4.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">4. Hệ thống xác thực thông tin. </t>
     </r>
@@ -496,6 +427,61 @@
   </si>
   <si>
     <t>Quản lí có thể sửa ca làm (xóa, thêm hoặc chỉnh sửa) dựa theo giờ làm thực của nhân viên, tính lương, check in.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Hệ thống chuyển tiếp vào trang danh mục nhân viên, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Actor xem cửa sổ đã hiển thị  use case kết thúc tại đây. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Actor chọn xem thông tin nhân viên. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>A1, A2, A3.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Actor chọn nhân viên muốn xóa</t>
+  </si>
+  <si>
+    <t>2. Actor nhấn vào nút xóa</t>
+  </si>
+  <si>
+    <t>3. Hệ thống hiện bảng xác nhận xóa</t>
+  </si>
+  <si>
+    <t>5. Hệ thống xóa nhân viên khỏi CSDL.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. Actor nhấn nút xác nhận xóa. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>A4</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Actor nhấn nút hủy</t>
+  </si>
+  <si>
+    <t>2. Quay trở về trang danh mục nhân viên</t>
   </si>
 </sst>
 </file>
@@ -620,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -659,6 +645,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -668,52 +684,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,23 +728,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>110288</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>396213</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>116262</xdr:rowOff>
+      <xdr:rowOff>76855</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DECA50B3-BC91-4626-BB13-7E50B974C0A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20BA0443-6687-4E5D-9843-6F61D277D1BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -768,8 +760,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="16613605"/>
-          <a:ext cx="9123946" cy="8638631"/>
+          <a:off x="2398295" y="18296021"/>
+          <a:ext cx="6628571" cy="6790476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1127,67 +1119,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C2621A-69EC-42B6-924F-E3471F86D7A7}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="B56" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" style="1" customWidth="1"/>
     <col min="2" max="2" width="41" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="40.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
-    </row>
-    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1197,71 +1189,71 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="27"/>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="27"/>
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="27"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:3" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="26"/>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="C15" s="24"/>
+    </row>
+    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="27"/>
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1269,62 +1261,62 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+    <row r="17" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27"/>
       <c r="B17" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+    <row r="18" spans="1:3" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27"/>
       <c r="B20" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C20" s="6"/>
     </row>
-    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
+    <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-    </row>
-    <row r="24" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="26"/>
-    </row>
-    <row r="25" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+    </row>
+    <row r="24" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="27"/>
+      <c r="B24" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27"/>
       <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1332,208 +1324,259 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27"/>
       <c r="B26" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+    <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27"/>
       <c r="B28" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+    <row r="29" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27"/>
       <c r="B29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="27"/>
       <c r="B30" s="2"/>
       <c r="C30" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27"/>
       <c r="B31" s="3"/>
       <c r="C31" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27"/>
+      <c r="B33" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="18"/>
+    </row>
+    <row r="34" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="27"/>
+      <c r="B34" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="27"/>
+      <c r="B35" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27"/>
+      <c r="B36" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="27"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27"/>
+      <c r="B38" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="16"/>
+    </row>
+    <row r="39" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="27"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+    </row>
+    <row r="41" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="27"/>
+      <c r="B41" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="16"/>
+    </row>
+    <row r="42" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27"/>
+      <c r="B42" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="27"/>
+      <c r="B43" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="16"/>
+    </row>
+    <row r="44" spans="1:3" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="24"/>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27"/>
+      <c r="B47" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="24"/>
+    </row>
+    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="20"/>
+    </row>
+    <row r="49" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-    </row>
-    <row r="33" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="23"/>
-    </row>
-    <row r="34" spans="1:3" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="2" t="s">
+      <c r="C49" s="20"/>
+    </row>
+    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="20"/>
+    </row>
+    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="20"/>
+    </row>
+    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="2" t="s">
+      <c r="C52" s="20"/>
+    </row>
+    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="20"/>
+    </row>
+    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-    </row>
-    <row r="38" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C38" s="26"/>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="26"/>
-    </row>
-    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-    </row>
-    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="23"/>
-    </row>
-    <row r="42" spans="1:3" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="23"/>
-    </row>
-    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="23"/>
-    </row>
-    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="23"/>
-    </row>
-    <row r="45" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="23"/>
-    </row>
-    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="C54" s="20"/>
+    </row>
+    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B47" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="23"/>
-    </row>
-    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="22">
+      <c r="B55" s="29">
         <v>44154</v>
       </c>
-      <c r="C48" s="23"/>
+      <c r="C55" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="A15:A45"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A15:A37"/>
-    <mergeCell ref="B37:C37"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B23:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1545,451 +1588,451 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734B381B-EDB8-4874-9EC9-0431D31E0CB1}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" zoomScale="86" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScale="86" workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="83.28515625" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="34.88671875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="53.88671875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="83.33203125" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="31"/>
-    </row>
-    <row r="3" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="30"/>
+    </row>
+    <row r="3" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="31"/>
-    </row>
-    <row r="4" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="30"/>
+    </row>
+    <row r="4" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="31"/>
-    </row>
-    <row r="5" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="30"/>
+    </row>
+    <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
       <c r="B7" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C7" s="9"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="36"/>
       <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="36"/>
       <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="36"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="36"/>
+      <c r="B11" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="36"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="36"/>
+      <c r="B13" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="36"/>
       <c r="B14" s="10"/>
       <c r="C14" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="36"/>
       <c r="B15" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="36"/>
       <c r="B16" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="36"/>
       <c r="B17" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="36"/>
       <c r="B18" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="36"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="36"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="36"/>
       <c r="B22" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="36"/>
       <c r="B23" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="36"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="36"/>
       <c r="B25" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
+    <row r="26" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="36"/>
       <c r="B26" s="8"/>
       <c r="C26" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="30"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="36"/>
+      <c r="B27" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="33"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="36"/>
       <c r="B28" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="36"/>
       <c r="B29" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="36"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="36"/>
       <c r="B31" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="30"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="36"/>
+      <c r="B32" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="33"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="36"/>
       <c r="B33" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="36"/>
       <c r="B34" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C34" s="10"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="36"/>
       <c r="B35" s="8"/>
       <c r="C35" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="36"/>
       <c r="B36" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="36"/>
       <c r="B37" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C37" s="8"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="36"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
-      <c r="B39" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="30"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="36"/>
+      <c r="B39" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="33"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="36"/>
       <c r="B40" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="36"/>
       <c r="B41" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C41" s="8"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="36"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="28"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="36"/>
       <c r="B43" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="36"/>
       <c r="B44" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="36"/>
       <c r="B45" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="36"/>
       <c r="B46" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="36"/>
       <c r="B47" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C47" s="8"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="36"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="36"/>
       <c r="B49" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="1:3" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28"/>
+    <row r="50" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="36"/>
       <c r="B50" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="36"/>
       <c r="B51" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="36"/>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="33" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="36"/>
       <c r="B53" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="36"/>
       <c r="B54" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="36"/>
       <c r="B55" s="9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="36"/>
       <c r="B56" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="36"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="28"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="36"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="14" t="s">
         <v>16</v>
       </c>
@@ -1998,108 +2041,113 @@
       </c>
       <c r="C59" s="8"/>
     </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="31"/>
-    </row>
-    <row r="61" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="30"/>
+    </row>
+    <row r="61" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="34" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C61" s="35"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B62" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="31"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C62" s="30"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C63" s="8"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="30"/>
+    </row>
+    <row r="65" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B64" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="31"/>
-    </row>
-    <row r="65" spans="1:3" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="B65" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" s="8"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C65" s="8"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="B66" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" s="31"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C66" s="32"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B67" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="31"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="30"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
     </row>
-    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15"/>
     </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15"/>
     </row>
-    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15"/>
     </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15"/>
     </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="82.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="49.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="49.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="82.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A6:A20"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A21:A58"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B64:C64"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C67"/>
@@ -2111,11 +2159,6 @@
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B61:C61"/>
-    <mergeCell ref="A6:A20"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A21:A58"/>
-    <mergeCell ref="B62:C62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>